<commit_message>
updated the coords file
</commit_message>
<xml_diff>
--- a/Documentation/R5 Coords.xlsx
+++ b/Documentation/R5 Coords.xlsx
@@ -1,24 +1,30 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="27610"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documents\Game_RPG_HTML\Game_RPG_Adventure\Documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/koen/Documents/GitHub/Game_RPG_Adventure/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAA55BA1-655C-4435-A6EF-EBFBA4A6DC0F}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{512C78F3-A0C6-4ABF-A448-CB69E8D98F3B}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="27320" windowHeight="13460" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
     <sheet name="V2" sheetId="2" r:id="rId2"/>
+    <sheet name="Converted to numbers" sheetId="4" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -31,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="93">
   <si>
     <t xml:space="preserve">Plain </t>
   </si>
@@ -315,7 +321,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -927,7 +933,7 @@
     <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="84">
+  <cellXfs count="85">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="4" fillId="10" borderId="0" xfId="9"/>
@@ -1163,6 +1169,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="16">
@@ -1178,10 +1187,10 @@
     <cellStyle name="Accent2" xfId="4" builtinId="33"/>
     <cellStyle name="Accent4" xfId="12" builtinId="41"/>
     <cellStyle name="Accent6" xfId="9" builtinId="49"/>
-    <cellStyle name="Goed" xfId="1" builtinId="26"/>
-    <cellStyle name="Neutraal" xfId="11" builtinId="28"/>
-    <cellStyle name="Ongeldig" xfId="2" builtinId="27"/>
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
+    <cellStyle name="Neutral" xfId="11" builtinId="28"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1492,20 +1501,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E865CB17-64F7-4862-A25D-07AD5395119C}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="AH10" sqref="AH10:AH11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P4" sqref="P4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="13" width="6.7109375" customWidth="1"/>
-    <col min="18" max="28" width="5.7109375" customWidth="1"/>
+    <col min="2" max="13" width="6.6640625" customWidth="1"/>
+    <col min="18" max="28" width="5.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="83" t="s">
         <v>92</v>
       </c>
@@ -1515,7 +1524,7 @@
       <c r="E1" s="83"/>
       <c r="F1" s="82"/>
     </row>
-    <row r="2" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="83" t="s">
         <v>91</v>
       </c>
@@ -1531,7 +1540,7 @@
       <c r="K2" s="83"/>
       <c r="L2" s="83"/>
     </row>
-    <row r="3" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
       <c r="D3" s="7"/>
@@ -1563,7 +1572,7 @@
       <c r="AA3" s="7"/>
       <c r="AB3" s="12"/>
     </row>
-    <row r="4" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B4" s="8"/>
       <c r="C4" s="9"/>
       <c r="D4" s="51" t="s">
@@ -1619,7 +1628,7 @@
       <c r="AA4" s="9"/>
       <c r="AB4" s="13"/>
     </row>
-    <row r="5" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B5" s="8"/>
       <c r="C5" s="61" t="s">
         <v>61</v>
@@ -1683,7 +1692,7 @@
       </c>
       <c r="AB5" s="13"/>
     </row>
-    <row r="6" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B6" s="8"/>
       <c r="C6" s="63" t="s">
         <v>39</v>
@@ -1747,7 +1756,7 @@
       </c>
       <c r="AB6" s="13"/>
     </row>
-    <row r="7" spans="1:28" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="8"/>
       <c r="C7" s="63" t="s">
         <v>38</v>
@@ -1811,7 +1820,7 @@
       </c>
       <c r="AB7" s="13"/>
     </row>
-    <row r="8" spans="1:28" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="47" t="s">
         <v>14</v>
       </c>
@@ -1883,7 +1892,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="9" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="8"/>
       <c r="C9" s="63" t="s">
         <v>74</v>
@@ -1947,7 +1956,7 @@
       </c>
       <c r="AB9" s="13"/>
     </row>
-    <row r="10" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B10" s="8"/>
       <c r="C10" s="63" t="s">
         <v>73</v>
@@ -2008,7 +2017,7 @@
       </c>
       <c r="AB10" s="13"/>
     </row>
-    <row r="11" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B11" s="8"/>
       <c r="C11" s="54" t="s">
         <v>75</v>
@@ -2067,7 +2076,7 @@
       </c>
       <c r="AB11" s="13"/>
     </row>
-    <row r="12" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B12" s="8"/>
       <c r="C12" s="9"/>
       <c r="D12" s="54" t="s">
@@ -2118,7 +2127,7 @@
       <c r="AA12" s="9"/>
       <c r="AB12" s="13"/>
     </row>
-    <row r="13" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="8"/>
       <c r="C13" s="9"/>
       <c r="D13" s="9"/>
@@ -2143,7 +2152,7 @@
       <c r="AA13" s="9"/>
       <c r="AB13" s="13"/>
     </row>
-    <row r="14" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
       <c r="C14" s="11"/>
       <c r="D14" s="11"/>
@@ -2164,7 +2173,7 @@
       <c r="AA14" s="11"/>
       <c r="AB14" s="14"/>
     </row>
-    <row r="15" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B15" s="6"/>
       <c r="C15" s="7"/>
       <c r="D15" s="7"/>
@@ -2177,7 +2186,7 @@
       <c r="K15" s="7"/>
       <c r="L15" s="12"/>
     </row>
-    <row r="16" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B16" s="8"/>
       <c r="C16" s="9"/>
       <c r="D16" s="42"/>
@@ -2190,7 +2199,7 @@
       <c r="K16" s="9"/>
       <c r="L16" s="13"/>
     </row>
-    <row r="17" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B17" s="8"/>
       <c r="C17" s="42"/>
       <c r="D17" s="43"/>
@@ -2203,7 +2212,7 @@
       <c r="K17" s="29"/>
       <c r="L17" s="13"/>
     </row>
-    <row r="18" spans="2:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B18" s="8"/>
       <c r="C18" s="44"/>
       <c r="D18" s="43"/>
@@ -2216,7 +2225,7 @@
       <c r="K18" s="30"/>
       <c r="L18" s="13"/>
     </row>
-    <row r="19" spans="2:12" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:12" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B19" s="8"/>
       <c r="C19" s="36"/>
       <c r="D19" s="19"/>
@@ -2229,7 +2238,7 @@
       <c r="K19" s="33"/>
       <c r="L19" s="13"/>
     </row>
-    <row r="20" spans="2:12" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:12" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B20" s="38"/>
       <c r="C20" s="37"/>
       <c r="D20" s="19"/>
@@ -2242,7 +2251,7 @@
       <c r="K20" s="23"/>
       <c r="L20" s="25"/>
     </row>
-    <row r="21" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B21" s="8"/>
       <c r="C21" s="39"/>
       <c r="D21" s="19"/>
@@ -2255,7 +2264,7 @@
       <c r="K21" s="26"/>
       <c r="L21" s="13"/>
     </row>
-    <row r="22" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B22" s="8"/>
       <c r="C22" s="39"/>
       <c r="D22" s="37"/>
@@ -2268,7 +2277,7 @@
       <c r="K22" s="26"/>
       <c r="L22" s="13"/>
     </row>
-    <row r="23" spans="2:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:12" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B23" s="8"/>
       <c r="C23" s="41"/>
       <c r="D23" s="37"/>
@@ -2281,7 +2290,7 @@
       <c r="K23" s="16"/>
       <c r="L23" s="13"/>
     </row>
-    <row r="24" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B24" s="8"/>
       <c r="C24" s="9"/>
       <c r="D24" s="41"/>
@@ -2294,7 +2303,7 @@
       <c r="K24" s="9"/>
       <c r="L24" s="13"/>
     </row>
-    <row r="25" spans="2:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:12" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B25" s="8"/>
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
@@ -2307,7 +2316,7 @@
       <c r="K25" s="9"/>
       <c r="L25" s="13"/>
     </row>
-    <row r="26" spans="2:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" x14ac:dyDescent="0.2">
       <c r="B26" s="10"/>
       <c r="C26" s="11"/>
       <c r="D26" s="11"/>
@@ -2331,21 +2340,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{633D3A55-0251-4EBF-A0D1-C7B60468E582}">
-  <dimension ref="A1:BE23"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:BE46"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="AD12" sqref="AD12"/>
+    <sheetView zoomScale="60" zoomScaleNormal="70" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:V22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="6.5703125" customWidth="1"/>
+    <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="28" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="2" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="68"/>
       <c r="B2" s="68"/>
       <c r="C2" s="68"/>
@@ -2411,7 +2420,7 @@
       <c r="BD2" s="68"/>
       <c r="BE2" s="68"/>
     </row>
-    <row r="3" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="68"/>
       <c r="B3" s="68"/>
       <c r="C3" s="68"/>
@@ -2477,7 +2486,7 @@
       <c r="BD3" s="68"/>
       <c r="BE3" s="68"/>
     </row>
-    <row r="4" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="68"/>
       <c r="B4" s="68"/>
       <c r="C4" s="68"/>
@@ -2543,7 +2552,7 @@
       <c r="BD4" s="68"/>
       <c r="BE4" s="68"/>
     </row>
-    <row r="5" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="68"/>
       <c r="B5" s="68"/>
       <c r="C5" s="68"/>
@@ -2601,7 +2610,7 @@
       <c r="BD5" s="68"/>
       <c r="BE5" s="68"/>
     </row>
-    <row r="6" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="68"/>
       <c r="B6" s="68"/>
       <c r="C6" s="68"/>
@@ -2659,7 +2668,7 @@
       <c r="BD6" s="68"/>
       <c r="BE6" s="68"/>
     </row>
-    <row r="7" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="68"/>
       <c r="B7" s="68"/>
       <c r="C7" s="68"/>
@@ -2717,7 +2726,7 @@
       <c r="BD7" s="68"/>
       <c r="BE7" s="68"/>
     </row>
-    <row r="8" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="68"/>
       <c r="B8" s="68"/>
       <c r="C8" s="77" t="s">
@@ -2775,7 +2784,7 @@
       </c>
       <c r="BE8" s="68"/>
     </row>
-    <row r="9" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="68"/>
       <c r="B9" s="68"/>
       <c r="C9" s="77" t="s">
@@ -2833,7 +2842,7 @@
       </c>
       <c r="BE9" s="68"/>
     </row>
-    <row r="10" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="68"/>
       <c r="B10" s="77" t="s">
         <v>83</v>
@@ -2891,7 +2900,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="11" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="68"/>
       <c r="B11" s="77" t="s">
         <v>83</v>
@@ -2942,7 +2951,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="12" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="68"/>
       <c r="B12" s="77">
         <v>-10</v>
@@ -3072,7 +3081,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="68"/>
       <c r="B13" s="74" t="s">
         <v>83</v>
@@ -3128,15 +3137,15 @@
         <v>83</v>
       </c>
     </row>
-    <row r="14" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="68"/>
       <c r="B14" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="79" t="s">
+      <c r="C14" s="84" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="79"/>
+      <c r="D14" s="84"/>
       <c r="E14" s="78"/>
       <c r="F14" s="80"/>
       <c r="G14" s="80"/>
@@ -3192,7 +3201,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="15" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="68"/>
       <c r="B15" s="68"/>
       <c r="C15" s="76" t="s">
@@ -3254,7 +3263,7 @@
       </c>
       <c r="BE15" s="68"/>
     </row>
-    <row r="16" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="68"/>
       <c r="B16" s="68"/>
       <c r="C16" s="76" t="s">
@@ -3316,7 +3325,7 @@
       </c>
       <c r="BE16" s="68"/>
     </row>
-    <row r="17" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="68"/>
       <c r="B17" s="68"/>
       <c r="C17" s="68"/>
@@ -3378,7 +3387,7 @@
       <c r="BD17" s="68"/>
       <c r="BE17" s="68"/>
     </row>
-    <row r="18" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="68"/>
       <c r="B18" s="68"/>
       <c r="C18" s="68"/>
@@ -3440,7 +3449,7 @@
       <c r="BD18" s="68"/>
       <c r="BE18" s="68"/>
     </row>
-    <row r="19" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="68"/>
       <c r="B19" s="68"/>
       <c r="C19" s="68"/>
@@ -3502,7 +3511,7 @@
       <c r="BD19" s="68"/>
       <c r="BE19" s="68"/>
     </row>
-    <row r="20" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="68"/>
       <c r="B20" s="68"/>
       <c r="C20" s="68"/>
@@ -3572,7 +3581,7 @@
       <c r="BD20" s="68"/>
       <c r="BE20" s="68"/>
     </row>
-    <row r="21" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="68"/>
       <c r="B21" s="68"/>
       <c r="C21" s="68"/>
@@ -3642,7 +3651,7 @@
       <c r="BD21" s="68"/>
       <c r="BE21" s="68"/>
     </row>
-    <row r="22" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:57" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="68"/>
       <c r="B22" s="68"/>
       <c r="C22" s="68"/>
@@ -3712,11 +3721,1847 @@
       <c r="BD22" s="68"/>
       <c r="BE22" s="68"/>
     </row>
-    <row r="23" spans="1:57" ht="28.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="23" spans="1:57" ht="28.5" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="26" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="B26" s="68"/>
+      <c r="C26" s="68"/>
+      <c r="D26" s="68"/>
+      <c r="E26" s="68"/>
+      <c r="F26" s="68"/>
+      <c r="G26" s="68"/>
+      <c r="H26" s="68"/>
+      <c r="I26" s="68"/>
+      <c r="J26" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="K26" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="L26" s="74">
+        <v>10</v>
+      </c>
+      <c r="M26" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="N26" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="O26" s="68"/>
+      <c r="P26" s="68"/>
+      <c r="Q26" s="68"/>
+      <c r="R26" s="68"/>
+      <c r="S26" s="68"/>
+      <c r="T26" s="68"/>
+      <c r="U26" s="68"/>
+      <c r="V26" s="68"/>
+    </row>
+    <row r="27" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="B27" s="68"/>
+      <c r="C27" s="68"/>
+      <c r="D27" s="68"/>
+      <c r="E27" s="68"/>
+      <c r="F27" s="68"/>
+      <c r="G27" s="68"/>
+      <c r="H27" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="I27" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="J27" s="80"/>
+      <c r="K27" s="80"/>
+      <c r="L27" s="80">
+        <v>9</v>
+      </c>
+      <c r="M27" s="80"/>
+      <c r="N27" s="75"/>
+      <c r="O27" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="P27" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q27" s="68"/>
+      <c r="R27" s="68"/>
+      <c r="S27" s="68"/>
+      <c r="T27" s="68"/>
+      <c r="U27" s="68"/>
+      <c r="V27" s="68"/>
+    </row>
+    <row r="28" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="B28" s="68"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="68"/>
+      <c r="F28" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="G28" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="H28" s="77"/>
+      <c r="I28" s="74"/>
+      <c r="J28" s="80"/>
+      <c r="K28" s="80"/>
+      <c r="L28" s="80">
+        <v>8</v>
+      </c>
+      <c r="M28" s="80"/>
+      <c r="N28" s="75"/>
+      <c r="O28" s="75"/>
+      <c r="P28" s="75"/>
+      <c r="Q28" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="R28" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="S28" s="68"/>
+      <c r="T28" s="68"/>
+      <c r="U28" s="68"/>
+      <c r="V28" s="68"/>
+    </row>
+    <row r="29" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="B29" s="68"/>
+      <c r="C29" s="68"/>
+      <c r="D29" s="68"/>
+      <c r="E29" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="F29" s="77"/>
+      <c r="G29" s="77"/>
+      <c r="H29" s="77"/>
+      <c r="I29" s="74"/>
+      <c r="J29" s="80"/>
+      <c r="K29" s="80"/>
+      <c r="L29" s="80">
+        <v>7</v>
+      </c>
+      <c r="M29" s="80"/>
+      <c r="N29" s="80"/>
+      <c r="O29" s="75"/>
+      <c r="P29" s="75"/>
+      <c r="Q29" s="75"/>
+      <c r="R29" s="75"/>
+      <c r="S29" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="T29" s="68"/>
+      <c r="U29" s="68"/>
+      <c r="V29" s="68"/>
+    </row>
+    <row r="30" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="B30" s="68"/>
+      <c r="C30" s="68"/>
+      <c r="D30" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="E30" s="77"/>
+      <c r="F30" s="77"/>
+      <c r="G30" s="77"/>
+      <c r="H30" s="77"/>
+      <c r="I30" s="74"/>
+      <c r="J30" s="80"/>
+      <c r="K30" s="80"/>
+      <c r="L30" s="80">
+        <v>6</v>
+      </c>
+      <c r="M30" s="80"/>
+      <c r="N30" s="80"/>
+      <c r="O30" s="80"/>
+      <c r="P30" s="75"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="75"/>
+      <c r="S30" s="75"/>
+      <c r="T30" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="U30" s="68"/>
+      <c r="V30" s="68"/>
+    </row>
+    <row r="31" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="B31" s="68"/>
+      <c r="C31" s="68"/>
+      <c r="D31" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="E31" s="77"/>
+      <c r="F31" s="77"/>
+      <c r="G31" s="77"/>
+      <c r="H31" s="77"/>
+      <c r="I31" s="74"/>
+      <c r="J31" s="80"/>
+      <c r="K31" s="80"/>
+      <c r="L31" s="80">
+        <v>5</v>
+      </c>
+      <c r="M31" s="80"/>
+      <c r="N31" s="74"/>
+      <c r="O31" s="80"/>
+      <c r="P31" s="80"/>
+      <c r="Q31" s="80"/>
+      <c r="R31" s="75"/>
+      <c r="S31" s="75"/>
+      <c r="T31" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="U31" s="68"/>
+      <c r="V31" s="68"/>
+    </row>
+    <row r="32" spans="1:57" x14ac:dyDescent="0.2">
+      <c r="B32" s="68"/>
+      <c r="C32" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="77"/>
+      <c r="E32" s="77"/>
+      <c r="F32" s="77"/>
+      <c r="G32" s="77"/>
+      <c r="H32" s="77"/>
+      <c r="I32" s="74"/>
+      <c r="J32" s="74"/>
+      <c r="K32" s="74"/>
+      <c r="L32" s="74">
+        <v>4</v>
+      </c>
+      <c r="M32" s="80"/>
+      <c r="N32" s="74"/>
+      <c r="O32" s="74"/>
+      <c r="P32" s="74"/>
+      <c r="Q32" s="80"/>
+      <c r="R32" s="80"/>
+      <c r="S32" s="75"/>
+      <c r="T32" s="75"/>
+      <c r="U32" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="V32" s="68"/>
+    </row>
+    <row r="33" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B33" s="68"/>
+      <c r="C33" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="D33" s="77"/>
+      <c r="E33" s="77"/>
+      <c r="F33" s="77"/>
+      <c r="G33" s="77"/>
+      <c r="H33" s="74"/>
+      <c r="I33" s="74"/>
+      <c r="J33" s="74"/>
+      <c r="K33" s="74"/>
+      <c r="L33" s="74">
+        <v>3</v>
+      </c>
+      <c r="M33" s="74"/>
+      <c r="N33" s="74"/>
+      <c r="O33" s="74"/>
+      <c r="P33" s="74"/>
+      <c r="Q33" s="74"/>
+      <c r="R33" s="74"/>
+      <c r="S33" s="80"/>
+      <c r="T33" s="75"/>
+      <c r="U33" s="75" t="s">
+        <v>83</v>
+      </c>
+      <c r="V33" s="68"/>
+    </row>
+    <row r="34" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B34" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C34" s="77"/>
+      <c r="D34" s="77"/>
+      <c r="E34" s="77"/>
+      <c r="F34" s="77"/>
+      <c r="G34" s="74"/>
+      <c r="H34" s="74"/>
+      <c r="I34" s="74"/>
+      <c r="J34" s="74"/>
+      <c r="K34" s="74"/>
+      <c r="L34" s="74">
+        <v>2</v>
+      </c>
+      <c r="M34" s="74"/>
+      <c r="N34" s="74"/>
+      <c r="O34" s="74"/>
+      <c r="P34" s="74"/>
+      <c r="Q34" s="74"/>
+      <c r="R34" s="74"/>
+      <c r="S34" s="80"/>
+      <c r="T34" s="75"/>
+      <c r="U34" s="75"/>
+      <c r="V34" s="75" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B35" s="77" t="s">
+        <v>83</v>
+      </c>
+      <c r="C35" s="77"/>
+      <c r="D35" s="77"/>
+      <c r="E35" s="77"/>
+      <c r="F35" s="74"/>
+      <c r="G35" s="74"/>
+      <c r="H35" s="74"/>
+      <c r="I35" s="80"/>
+      <c r="J35" s="74"/>
+      <c r="K35" s="74"/>
+      <c r="L35" s="74">
+        <v>1</v>
+      </c>
+      <c r="M35" s="74"/>
+      <c r="N35" s="74"/>
+      <c r="O35" s="81"/>
+      <c r="P35" s="81"/>
+      <c r="Q35" s="2"/>
+      <c r="R35" s="2"/>
+      <c r="S35" s="2"/>
+      <c r="T35" s="2"/>
+      <c r="U35" s="2"/>
+      <c r="V35" s="75" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="36" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B36" s="77">
+        <v>-10</v>
+      </c>
+      <c r="C36" s="77">
+        <v>-9</v>
+      </c>
+      <c r="D36" s="77">
+        <v>-8</v>
+      </c>
+      <c r="E36" s="74">
+        <v>-7</v>
+      </c>
+      <c r="F36" s="74">
+        <v>-6</v>
+      </c>
+      <c r="G36" s="80">
+        <v>-5</v>
+      </c>
+      <c r="H36" s="80">
+        <v>-4</v>
+      </c>
+      <c r="I36" s="80">
+        <v>-3</v>
+      </c>
+      <c r="J36" s="74">
+        <v>-2</v>
+      </c>
+      <c r="K36" s="74">
+        <v>-1</v>
+      </c>
+      <c r="L36" s="74">
+        <v>0</v>
+      </c>
+      <c r="M36" s="74">
+        <v>1</v>
+      </c>
+      <c r="N36" s="74">
+        <v>2</v>
+      </c>
+      <c r="O36" s="80">
+        <v>3</v>
+      </c>
+      <c r="P36" s="80">
+        <v>4</v>
+      </c>
+      <c r="Q36" s="74">
+        <v>5</v>
+      </c>
+      <c r="R36" s="74">
+        <v>6</v>
+      </c>
+      <c r="S36" s="70">
+        <v>7</v>
+      </c>
+      <c r="T36" s="72">
+        <v>8</v>
+      </c>
+      <c r="U36" s="72">
+        <v>9</v>
+      </c>
+      <c r="V36" s="72">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="37" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B37" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="C37" s="74"/>
+      <c r="D37" s="74"/>
+      <c r="E37" s="74"/>
+      <c r="F37" s="80"/>
+      <c r="G37" s="80"/>
+      <c r="H37" s="80"/>
+      <c r="I37" s="80"/>
+      <c r="J37" s="80"/>
+      <c r="K37" s="74"/>
+      <c r="L37" s="74">
+        <v>-1</v>
+      </c>
+      <c r="M37" s="74"/>
+      <c r="N37" s="74"/>
+      <c r="O37" s="80"/>
+      <c r="P37" s="80"/>
+      <c r="Q37" s="74"/>
+      <c r="R37" s="74"/>
+      <c r="S37" s="72"/>
+      <c r="T37" s="4"/>
+      <c r="U37" s="4"/>
+      <c r="V37" s="73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="38" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B38" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="84" t="s">
+        <v>84</v>
+      </c>
+      <c r="D38" s="84"/>
+      <c r="E38" s="78"/>
+      <c r="F38" s="80"/>
+      <c r="G38" s="80"/>
+      <c r="H38" s="80"/>
+      <c r="I38" s="80"/>
+      <c r="J38" s="80"/>
+      <c r="K38" s="74"/>
+      <c r="L38" s="74">
+        <v>-2</v>
+      </c>
+      <c r="M38" s="74"/>
+      <c r="N38" s="74"/>
+      <c r="O38" s="80"/>
+      <c r="P38" s="80"/>
+      <c r="Q38" s="80"/>
+      <c r="R38" s="71"/>
+      <c r="S38" s="73"/>
+      <c r="T38" s="73"/>
+      <c r="U38" s="73"/>
+      <c r="V38" s="73" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="39" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B39" s="68"/>
+      <c r="C39" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="D39" s="76"/>
+      <c r="E39" s="78"/>
+      <c r="F39" s="74"/>
+      <c r="G39" s="74"/>
+      <c r="H39" s="74"/>
+      <c r="I39" s="81"/>
+      <c r="J39" s="80"/>
+      <c r="K39" s="80"/>
+      <c r="L39" s="74">
+        <v>-3</v>
+      </c>
+      <c r="M39" s="74"/>
+      <c r="N39" s="74"/>
+      <c r="O39" s="80"/>
+      <c r="P39" s="80"/>
+      <c r="Q39" s="72"/>
+      <c r="R39" s="73"/>
+      <c r="S39" s="73"/>
+      <c r="T39" s="73"/>
+      <c r="U39" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="V39" s="68"/>
+    </row>
+    <row r="40" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B40" s="68"/>
+      <c r="C40" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="D40" s="76"/>
+      <c r="E40" s="76"/>
+      <c r="F40" s="78"/>
+      <c r="G40" s="74"/>
+      <c r="H40" s="74"/>
+      <c r="I40" s="80"/>
+      <c r="J40" s="80"/>
+      <c r="K40" s="80"/>
+      <c r="L40" s="74">
+        <v>-4</v>
+      </c>
+      <c r="M40" s="74"/>
+      <c r="N40" s="74"/>
+      <c r="O40" s="80"/>
+      <c r="P40" s="80"/>
+      <c r="Q40" s="72"/>
+      <c r="R40" s="73"/>
+      <c r="S40" s="73"/>
+      <c r="T40" s="73"/>
+      <c r="U40" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="V40" s="68"/>
+    </row>
+    <row r="41" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B41" s="68"/>
+      <c r="C41" s="68"/>
+      <c r="D41" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="E41" s="76"/>
+      <c r="F41" s="78"/>
+      <c r="G41" s="74"/>
+      <c r="H41" s="74"/>
+      <c r="I41" s="80"/>
+      <c r="J41" s="80"/>
+      <c r="K41" s="80"/>
+      <c r="L41" s="74">
+        <v>-5</v>
+      </c>
+      <c r="M41" s="74"/>
+      <c r="N41" s="74"/>
+      <c r="O41" s="80"/>
+      <c r="P41" s="72"/>
+      <c r="Q41" s="73"/>
+      <c r="R41" s="73"/>
+      <c r="S41" s="73"/>
+      <c r="T41" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="U41" s="68"/>
+      <c r="V41" s="68"/>
+    </row>
+    <row r="42" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B42" s="68"/>
+      <c r="C42" s="68"/>
+      <c r="D42" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="E42" s="76"/>
+      <c r="F42" s="76"/>
+      <c r="G42" s="78"/>
+      <c r="H42" s="80"/>
+      <c r="I42" s="80"/>
+      <c r="J42" s="80"/>
+      <c r="K42" s="80"/>
+      <c r="L42" s="80">
+        <v>-6</v>
+      </c>
+      <c r="M42" s="74"/>
+      <c r="N42" s="74"/>
+      <c r="O42" s="80"/>
+      <c r="P42" s="72"/>
+      <c r="Q42" s="73"/>
+      <c r="R42" s="73"/>
+      <c r="S42" s="73"/>
+      <c r="T42" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="U42" s="68"/>
+      <c r="V42" s="68"/>
+    </row>
+    <row r="43" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B43" s="68"/>
+      <c r="C43" s="68"/>
+      <c r="D43" s="68"/>
+      <c r="E43" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="F43" s="76"/>
+      <c r="G43" s="76"/>
+      <c r="H43" s="78"/>
+      <c r="I43" s="78"/>
+      <c r="J43" s="78"/>
+      <c r="K43" s="80"/>
+      <c r="L43" s="80">
+        <v>-7</v>
+      </c>
+      <c r="M43" s="2"/>
+      <c r="N43" s="2"/>
+      <c r="O43" s="2"/>
+      <c r="P43" s="72"/>
+      <c r="Q43" s="73"/>
+      <c r="R43" s="73"/>
+      <c r="S43" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="T43" s="68"/>
+      <c r="U43" s="68"/>
+      <c r="V43" s="68"/>
+    </row>
+    <row r="44" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B44" s="68"/>
+      <c r="C44" s="68"/>
+      <c r="D44" s="68"/>
+      <c r="E44" s="68"/>
+      <c r="F44" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="G44" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="H44" s="76"/>
+      <c r="I44" s="76"/>
+      <c r="J44" s="76"/>
+      <c r="K44" s="78"/>
+      <c r="L44" s="80">
+        <v>-8</v>
+      </c>
+      <c r="M44" s="2"/>
+      <c r="N44" s="2"/>
+      <c r="O44" s="2"/>
+      <c r="P44" s="72"/>
+      <c r="Q44" s="73" t="s">
+        <v>83</v>
+      </c>
+      <c r="R44" s="71" t="s">
+        <v>83</v>
+      </c>
+      <c r="S44" s="68"/>
+      <c r="T44" s="68"/>
+      <c r="U44" s="68"/>
+      <c r="V44" s="68"/>
+    </row>
+    <row r="45" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B45" s="68"/>
+      <c r="C45" s="68"/>
+      <c r="D45" s="68"/>
+      <c r="E45" s="68"/>
+      <c r="F45" s="68"/>
+      <c r="G45" s="68"/>
+      <c r="H45" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="I45" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="J45" s="76"/>
+      <c r="K45" s="76"/>
+      <c r="L45" s="78">
+        <v>-9</v>
+      </c>
+      <c r="M45" s="76"/>
+      <c r="N45" s="76"/>
+      <c r="O45" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="P45" s="72" t="s">
+        <v>83</v>
+      </c>
+      <c r="Q45" s="68"/>
+      <c r="R45" s="68"/>
+      <c r="S45" s="68"/>
+      <c r="T45" s="68"/>
+      <c r="U45" s="68"/>
+      <c r="V45" s="68"/>
+    </row>
+    <row r="46" spans="2:22" x14ac:dyDescent="0.2">
+      <c r="B46" s="68"/>
+      <c r="C46" s="68"/>
+      <c r="D46" s="68"/>
+      <c r="E46" s="68"/>
+      <c r="F46" s="68"/>
+      <c r="G46" s="68"/>
+      <c r="H46" s="68"/>
+      <c r="I46" s="68"/>
+      <c r="J46" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="K46" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="L46" s="76">
+        <v>-10</v>
+      </c>
+      <c r="M46" s="78" t="s">
+        <v>83</v>
+      </c>
+      <c r="N46" s="76" t="s">
+        <v>83</v>
+      </c>
+      <c r="O46" s="68"/>
+      <c r="P46" s="68"/>
+      <c r="Q46" s="68"/>
+      <c r="R46" s="68"/>
+      <c r="S46" s="68"/>
+      <c r="T46" s="68"/>
+      <c r="U46" s="68"/>
+      <c r="V46" s="68"/>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C38:D38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:U21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A1" s="68"/>
+      <c r="B1" s="68"/>
+      <c r="C1" s="68"/>
+      <c r="D1" s="68"/>
+      <c r="E1" s="68"/>
+      <c r="F1" s="68"/>
+      <c r="G1" s="68"/>
+      <c r="H1" s="68"/>
+      <c r="I1" s="74">
+        <v>1</v>
+      </c>
+      <c r="J1" s="74">
+        <v>1</v>
+      </c>
+      <c r="K1" s="74">
+        <v>1</v>
+      </c>
+      <c r="L1" s="74">
+        <v>1</v>
+      </c>
+      <c r="M1" s="75">
+        <v>2</v>
+      </c>
+      <c r="N1" s="68"/>
+      <c r="O1" s="68"/>
+      <c r="P1" s="68"/>
+      <c r="Q1" s="68"/>
+      <c r="R1" s="68"/>
+      <c r="S1" s="68"/>
+      <c r="T1" s="68"/>
+      <c r="U1" s="68"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" s="68"/>
+      <c r="B2" s="68"/>
+      <c r="C2" s="68"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="68"/>
+      <c r="F2" s="68"/>
+      <c r="G2" s="77">
+        <v>6</v>
+      </c>
+      <c r="H2" s="74">
+        <v>1</v>
+      </c>
+      <c r="I2" s="80">
+        <v>0</v>
+      </c>
+      <c r="J2" s="80">
+        <v>0</v>
+      </c>
+      <c r="K2" s="80">
+        <v>0</v>
+      </c>
+      <c r="L2" s="80">
+        <v>0</v>
+      </c>
+      <c r="M2" s="75">
+        <v>2</v>
+      </c>
+      <c r="N2" s="75">
+        <v>2</v>
+      </c>
+      <c r="O2" s="75">
+        <v>2</v>
+      </c>
+      <c r="P2" s="68"/>
+      <c r="Q2" s="68"/>
+      <c r="R2" s="68"/>
+      <c r="S2" s="68"/>
+      <c r="T2" s="68"/>
+      <c r="U2" s="68"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3" s="68"/>
+      <c r="B3" s="68"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="71">
+        <v>4</v>
+      </c>
+      <c r="F3" s="77">
+        <v>6</v>
+      </c>
+      <c r="G3" s="77">
+        <v>6</v>
+      </c>
+      <c r="H3" s="74">
+        <v>1</v>
+      </c>
+      <c r="I3" s="80">
+        <v>0</v>
+      </c>
+      <c r="J3" s="80">
+        <v>0</v>
+      </c>
+      <c r="K3" s="80">
+        <v>0</v>
+      </c>
+      <c r="L3" s="80">
+        <v>0</v>
+      </c>
+      <c r="M3" s="75">
+        <v>2</v>
+      </c>
+      <c r="N3" s="75">
+        <v>2</v>
+      </c>
+      <c r="O3" s="75">
+        <v>2</v>
+      </c>
+      <c r="P3" s="75">
+        <v>2</v>
+      </c>
+      <c r="Q3" s="71">
+        <v>4</v>
+      </c>
+      <c r="R3" s="68"/>
+      <c r="S3" s="68"/>
+      <c r="T3" s="68"/>
+      <c r="U3" s="68"/>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4" s="68"/>
+      <c r="B4" s="68"/>
+      <c r="C4" s="68"/>
+      <c r="D4" s="77">
+        <v>6</v>
+      </c>
+      <c r="E4" s="77">
+        <v>6</v>
+      </c>
+      <c r="F4" s="77">
+        <v>6</v>
+      </c>
+      <c r="G4" s="77">
+        <v>6</v>
+      </c>
+      <c r="H4" s="74">
+        <v>1</v>
+      </c>
+      <c r="I4" s="80">
+        <v>0</v>
+      </c>
+      <c r="J4" s="80">
+        <v>0</v>
+      </c>
+      <c r="K4" s="80">
+        <v>0</v>
+      </c>
+      <c r="L4" s="80">
+        <v>0</v>
+      </c>
+      <c r="M4" s="80">
+        <v>0</v>
+      </c>
+      <c r="N4" s="75">
+        <v>2</v>
+      </c>
+      <c r="O4" s="75">
+        <v>2</v>
+      </c>
+      <c r="P4" s="75">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="75">
+        <v>2</v>
+      </c>
+      <c r="R4" s="75">
+        <v>2</v>
+      </c>
+      <c r="S4" s="68"/>
+      <c r="T4" s="68"/>
+      <c r="U4" s="68"/>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5" s="68"/>
+      <c r="B5" s="68"/>
+      <c r="C5" s="71">
+        <v>4</v>
+      </c>
+      <c r="D5" s="77">
+        <v>6</v>
+      </c>
+      <c r="E5" s="77">
+        <v>6</v>
+      </c>
+      <c r="F5" s="77">
+        <v>6</v>
+      </c>
+      <c r="G5" s="77">
+        <v>6</v>
+      </c>
+      <c r="H5" s="74">
+        <v>1</v>
+      </c>
+      <c r="I5" s="80">
+        <v>0</v>
+      </c>
+      <c r="J5" s="80">
+        <v>0</v>
+      </c>
+      <c r="K5" s="80">
+        <v>0</v>
+      </c>
+      <c r="L5" s="80">
+        <v>0</v>
+      </c>
+      <c r="M5" s="80">
+        <v>0</v>
+      </c>
+      <c r="N5" s="80">
+        <v>0</v>
+      </c>
+      <c r="O5" s="75">
+        <v>2</v>
+      </c>
+      <c r="P5" s="75">
+        <v>2</v>
+      </c>
+      <c r="Q5" s="75">
+        <v>2</v>
+      </c>
+      <c r="R5" s="75">
+        <v>2</v>
+      </c>
+      <c r="S5" s="71">
+        <v>4</v>
+      </c>
+      <c r="T5" s="68"/>
+      <c r="U5" s="68"/>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6" s="68"/>
+      <c r="B6" s="68"/>
+      <c r="C6" s="77">
+        <v>6</v>
+      </c>
+      <c r="D6" s="77">
+        <v>6</v>
+      </c>
+      <c r="E6" s="77">
+        <v>6</v>
+      </c>
+      <c r="F6" s="77">
+        <v>6</v>
+      </c>
+      <c r="G6" s="77">
+        <v>6</v>
+      </c>
+      <c r="H6" s="74">
+        <v>1</v>
+      </c>
+      <c r="I6" s="80">
+        <v>0</v>
+      </c>
+      <c r="J6" s="80">
+        <v>0</v>
+      </c>
+      <c r="K6" s="80">
+        <v>0</v>
+      </c>
+      <c r="L6" s="80">
+        <v>0</v>
+      </c>
+      <c r="M6" s="74">
+        <v>1</v>
+      </c>
+      <c r="N6" s="80">
+        <v>0</v>
+      </c>
+      <c r="O6" s="80">
+        <v>0</v>
+      </c>
+      <c r="P6" s="80">
+        <v>0</v>
+      </c>
+      <c r="Q6" s="75">
+        <v>2</v>
+      </c>
+      <c r="R6" s="75">
+        <v>2</v>
+      </c>
+      <c r="S6" s="75">
+        <v>2</v>
+      </c>
+      <c r="T6" s="68"/>
+      <c r="U6" s="68"/>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7" s="68"/>
+      <c r="B7" s="77">
+        <v>6</v>
+      </c>
+      <c r="C7" s="77">
+        <v>6</v>
+      </c>
+      <c r="D7" s="77">
+        <v>6</v>
+      </c>
+      <c r="E7" s="77">
+        <v>6</v>
+      </c>
+      <c r="F7" s="77">
+        <v>6</v>
+      </c>
+      <c r="G7" s="77">
+        <v>6</v>
+      </c>
+      <c r="H7" s="74">
+        <v>1</v>
+      </c>
+      <c r="I7" s="74">
+        <v>1</v>
+      </c>
+      <c r="J7" s="74">
+        <v>1</v>
+      </c>
+      <c r="K7" s="74">
+        <v>1</v>
+      </c>
+      <c r="L7" s="80">
+        <v>0</v>
+      </c>
+      <c r="M7" s="74">
+        <v>1</v>
+      </c>
+      <c r="N7" s="74">
+        <v>1</v>
+      </c>
+      <c r="O7" s="74">
+        <v>1</v>
+      </c>
+      <c r="P7" s="80">
+        <v>0</v>
+      </c>
+      <c r="Q7" s="80">
+        <v>0</v>
+      </c>
+      <c r="R7" s="75">
+        <v>2</v>
+      </c>
+      <c r="S7" s="75">
+        <v>2</v>
+      </c>
+      <c r="T7" s="75">
+        <v>2</v>
+      </c>
+      <c r="U7" s="68"/>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8" s="68"/>
+      <c r="B8" s="77">
+        <v>6</v>
+      </c>
+      <c r="C8" s="77">
+        <v>6</v>
+      </c>
+      <c r="D8" s="77">
+        <v>6</v>
+      </c>
+      <c r="E8" s="77">
+        <v>6</v>
+      </c>
+      <c r="F8" s="77">
+        <v>6</v>
+      </c>
+      <c r="G8" s="74">
+        <v>1</v>
+      </c>
+      <c r="H8" s="74">
+        <v>1</v>
+      </c>
+      <c r="I8" s="74">
+        <v>1</v>
+      </c>
+      <c r="J8" s="74">
+        <v>1</v>
+      </c>
+      <c r="K8" s="74">
+        <v>1</v>
+      </c>
+      <c r="L8" s="74">
+        <v>1</v>
+      </c>
+      <c r="M8" s="74">
+        <v>1</v>
+      </c>
+      <c r="N8" s="74">
+        <v>1</v>
+      </c>
+      <c r="O8" s="74">
+        <v>1</v>
+      </c>
+      <c r="P8" s="74">
+        <v>1</v>
+      </c>
+      <c r="Q8" s="74">
+        <v>1</v>
+      </c>
+      <c r="R8" s="80">
+        <v>0</v>
+      </c>
+      <c r="S8" s="75">
+        <v>2</v>
+      </c>
+      <c r="T8" s="75">
+        <v>2</v>
+      </c>
+      <c r="U8" s="68"/>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9" s="77">
+        <v>6</v>
+      </c>
+      <c r="B9" s="77">
+        <v>6</v>
+      </c>
+      <c r="C9" s="77">
+        <v>6</v>
+      </c>
+      <c r="D9" s="77">
+        <v>6</v>
+      </c>
+      <c r="E9" s="77">
+        <v>6</v>
+      </c>
+      <c r="F9" s="74">
+        <v>1</v>
+      </c>
+      <c r="G9" s="74">
+        <v>1</v>
+      </c>
+      <c r="H9" s="74">
+        <v>1</v>
+      </c>
+      <c r="I9" s="74">
+        <v>1</v>
+      </c>
+      <c r="J9" s="74">
+        <v>1</v>
+      </c>
+      <c r="K9" s="74">
+        <v>1</v>
+      </c>
+      <c r="L9" s="74">
+        <v>1</v>
+      </c>
+      <c r="M9" s="74">
+        <v>1</v>
+      </c>
+      <c r="N9" s="74">
+        <v>1</v>
+      </c>
+      <c r="O9" s="74">
+        <v>1</v>
+      </c>
+      <c r="P9" s="74">
+        <v>1</v>
+      </c>
+      <c r="Q9" s="74">
+        <v>1</v>
+      </c>
+      <c r="R9" s="80">
+        <v>0</v>
+      </c>
+      <c r="S9" s="75">
+        <v>2</v>
+      </c>
+      <c r="T9" s="75">
+        <v>2</v>
+      </c>
+      <c r="U9" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A10" s="77">
+        <v>6</v>
+      </c>
+      <c r="B10" s="77">
+        <v>6</v>
+      </c>
+      <c r="C10" s="77">
+        <v>6</v>
+      </c>
+      <c r="D10" s="77">
+        <v>6</v>
+      </c>
+      <c r="E10" s="74">
+        <v>1</v>
+      </c>
+      <c r="F10" s="74">
+        <v>1</v>
+      </c>
+      <c r="G10" s="74">
+        <v>1</v>
+      </c>
+      <c r="H10" s="80">
+        <v>0</v>
+      </c>
+      <c r="I10" s="74">
+        <v>1</v>
+      </c>
+      <c r="J10" s="74">
+        <v>1</v>
+      </c>
+      <c r="K10" s="74">
+        <v>1</v>
+      </c>
+      <c r="L10" s="74">
+        <v>1</v>
+      </c>
+      <c r="M10" s="74">
+        <v>1</v>
+      </c>
+      <c r="N10" s="81">
+        <v>0</v>
+      </c>
+      <c r="O10" s="81">
+        <v>0</v>
+      </c>
+      <c r="P10" s="2">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="2">
+        <v>1</v>
+      </c>
+      <c r="R10" s="2">
+        <v>1</v>
+      </c>
+      <c r="S10" s="2">
+        <v>1</v>
+      </c>
+      <c r="T10" s="2">
+        <v>1</v>
+      </c>
+      <c r="U10" s="75">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A11" s="77">
+        <v>6</v>
+      </c>
+      <c r="B11" s="77">
+        <v>6</v>
+      </c>
+      <c r="C11" s="77">
+        <v>6</v>
+      </c>
+      <c r="D11" s="74">
+        <v>1</v>
+      </c>
+      <c r="E11" s="74">
+        <v>1</v>
+      </c>
+      <c r="F11" s="80">
+        <v>0</v>
+      </c>
+      <c r="G11" s="80">
+        <v>0</v>
+      </c>
+      <c r="H11" s="80">
+        <v>0</v>
+      </c>
+      <c r="I11" s="74">
+        <v>1</v>
+      </c>
+      <c r="J11" s="74">
+        <v>1</v>
+      </c>
+      <c r="K11" s="74">
+        <v>1</v>
+      </c>
+      <c r="L11" s="74">
+        <v>1</v>
+      </c>
+      <c r="M11" s="74">
+        <v>1</v>
+      </c>
+      <c r="N11" s="80">
+        <v>0</v>
+      </c>
+      <c r="O11" s="80">
+        <v>0</v>
+      </c>
+      <c r="P11" s="74">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="74">
+        <v>1</v>
+      </c>
+      <c r="R11" s="70">
+        <v>10</v>
+      </c>
+      <c r="S11" s="72">
+        <v>9</v>
+      </c>
+      <c r="T11" s="72">
+        <v>9</v>
+      </c>
+      <c r="U11" s="72">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A12" s="74">
+        <v>1</v>
+      </c>
+      <c r="B12" s="74">
+        <v>1</v>
+      </c>
+      <c r="C12" s="74">
+        <v>1</v>
+      </c>
+      <c r="D12" s="74">
+        <v>1</v>
+      </c>
+      <c r="E12" s="80">
+        <v>0</v>
+      </c>
+      <c r="F12" s="80">
+        <v>0</v>
+      </c>
+      <c r="G12" s="80">
+        <v>0</v>
+      </c>
+      <c r="H12" s="80">
+        <v>0</v>
+      </c>
+      <c r="I12" s="80">
+        <v>0</v>
+      </c>
+      <c r="J12" s="74">
+        <v>1</v>
+      </c>
+      <c r="K12" s="74">
+        <v>1</v>
+      </c>
+      <c r="L12" s="74">
+        <v>1</v>
+      </c>
+      <c r="M12" s="74">
+        <v>1</v>
+      </c>
+      <c r="N12" s="80">
+        <v>0</v>
+      </c>
+      <c r="O12" s="80">
+        <v>0</v>
+      </c>
+      <c r="P12" s="74">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="74">
+        <v>1</v>
+      </c>
+      <c r="R12" s="72">
+        <v>9</v>
+      </c>
+      <c r="S12" s="4">
+        <v>3</v>
+      </c>
+      <c r="T12" s="4">
+        <v>3</v>
+      </c>
+      <c r="U12" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A13" s="74">
+        <v>1</v>
+      </c>
+      <c r="B13" s="79">
+        <v>7</v>
+      </c>
+      <c r="C13" s="79">
+        <v>7</v>
+      </c>
+      <c r="D13" s="78">
+        <v>8</v>
+      </c>
+      <c r="E13" s="80">
+        <v>0</v>
+      </c>
+      <c r="F13" s="80">
+        <v>0</v>
+      </c>
+      <c r="G13" s="80">
+        <v>0</v>
+      </c>
+      <c r="H13" s="80">
+        <v>0</v>
+      </c>
+      <c r="I13" s="80">
+        <v>0</v>
+      </c>
+      <c r="J13" s="74">
+        <v>1</v>
+      </c>
+      <c r="K13" s="74">
+        <v>1</v>
+      </c>
+      <c r="L13" s="74">
+        <v>1</v>
+      </c>
+      <c r="M13" s="74">
+        <v>1</v>
+      </c>
+      <c r="N13" s="80">
+        <v>0</v>
+      </c>
+      <c r="O13" s="80">
+        <v>0</v>
+      </c>
+      <c r="P13" s="80">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="71">
+        <v>4</v>
+      </c>
+      <c r="R13" s="73">
+        <v>3</v>
+      </c>
+      <c r="S13" s="73">
+        <v>3</v>
+      </c>
+      <c r="T13" s="73">
+        <v>3</v>
+      </c>
+      <c r="U13" s="73">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A14" s="68"/>
+      <c r="B14" s="76">
+        <v>5</v>
+      </c>
+      <c r="C14" s="76">
+        <v>5</v>
+      </c>
+      <c r="D14" s="78">
+        <v>8</v>
+      </c>
+      <c r="E14" s="74">
+        <v>1</v>
+      </c>
+      <c r="F14" s="74">
+        <v>1</v>
+      </c>
+      <c r="G14" s="74">
+        <v>1</v>
+      </c>
+      <c r="H14" s="81">
+        <v>0</v>
+      </c>
+      <c r="I14" s="80">
+        <v>0</v>
+      </c>
+      <c r="J14" s="80">
+        <v>0</v>
+      </c>
+      <c r="K14" s="74">
+        <v>1</v>
+      </c>
+      <c r="L14" s="74">
+        <v>1</v>
+      </c>
+      <c r="M14" s="74">
+        <v>1</v>
+      </c>
+      <c r="N14" s="80">
+        <v>0</v>
+      </c>
+      <c r="O14" s="80">
+        <v>0</v>
+      </c>
+      <c r="P14" s="72">
+        <v>9</v>
+      </c>
+      <c r="Q14" s="73">
+        <v>3</v>
+      </c>
+      <c r="R14" s="73">
+        <v>3</v>
+      </c>
+      <c r="S14" s="73">
+        <v>3</v>
+      </c>
+      <c r="T14" s="73">
+        <v>3</v>
+      </c>
+      <c r="U14" s="68"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A15" s="68"/>
+      <c r="B15" s="76">
+        <v>5</v>
+      </c>
+      <c r="C15" s="76">
+        <v>5</v>
+      </c>
+      <c r="D15" s="76">
+        <v>5</v>
+      </c>
+      <c r="E15" s="78">
+        <v>8</v>
+      </c>
+      <c r="F15" s="74">
+        <v>1</v>
+      </c>
+      <c r="G15" s="74">
+        <v>1</v>
+      </c>
+      <c r="H15" s="80">
+        <v>0</v>
+      </c>
+      <c r="I15" s="80">
+        <v>0</v>
+      </c>
+      <c r="J15" s="80">
+        <v>0</v>
+      </c>
+      <c r="K15" s="74">
+        <v>1</v>
+      </c>
+      <c r="L15" s="74">
+        <v>1</v>
+      </c>
+      <c r="M15" s="74">
+        <v>1</v>
+      </c>
+      <c r="N15" s="80">
+        <v>0</v>
+      </c>
+      <c r="O15" s="80">
+        <v>0</v>
+      </c>
+      <c r="P15" s="72">
+        <v>9</v>
+      </c>
+      <c r="Q15" s="73">
+        <v>3</v>
+      </c>
+      <c r="R15" s="73">
+        <v>3</v>
+      </c>
+      <c r="S15" s="73">
+        <v>3</v>
+      </c>
+      <c r="T15" s="73">
+        <v>3</v>
+      </c>
+      <c r="U15" s="68"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A16" s="68"/>
+      <c r="B16" s="68"/>
+      <c r="C16" s="76">
+        <v>5</v>
+      </c>
+      <c r="D16" s="76">
+        <v>5</v>
+      </c>
+      <c r="E16" s="78">
+        <v>8</v>
+      </c>
+      <c r="F16" s="74">
+        <v>1</v>
+      </c>
+      <c r="G16" s="74">
+        <v>1</v>
+      </c>
+      <c r="H16" s="80">
+        <v>0</v>
+      </c>
+      <c r="I16" s="80">
+        <v>0</v>
+      </c>
+      <c r="J16" s="80">
+        <v>0</v>
+      </c>
+      <c r="K16" s="74">
+        <v>1</v>
+      </c>
+      <c r="L16" s="74">
+        <v>1</v>
+      </c>
+      <c r="M16" s="74">
+        <v>1</v>
+      </c>
+      <c r="N16" s="80">
+        <v>0</v>
+      </c>
+      <c r="O16" s="72">
+        <v>9</v>
+      </c>
+      <c r="P16" s="73">
+        <v>3</v>
+      </c>
+      <c r="Q16" s="73">
+        <v>3</v>
+      </c>
+      <c r="R16" s="73">
+        <v>3</v>
+      </c>
+      <c r="S16" s="73">
+        <v>3</v>
+      </c>
+      <c r="T16" s="68"/>
+      <c r="U16" s="68"/>
+    </row>
+    <row r="17" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A17" s="68"/>
+      <c r="B17" s="68"/>
+      <c r="C17" s="71">
+        <v>4</v>
+      </c>
+      <c r="D17" s="76">
+        <v>5</v>
+      </c>
+      <c r="E17" s="76">
+        <v>5</v>
+      </c>
+      <c r="F17" s="78">
+        <v>8</v>
+      </c>
+      <c r="G17" s="80">
+        <v>0</v>
+      </c>
+      <c r="H17" s="80">
+        <v>0</v>
+      </c>
+      <c r="I17" s="80">
+        <v>0</v>
+      </c>
+      <c r="J17" s="80">
+        <v>0</v>
+      </c>
+      <c r="K17" s="80">
+        <v>0</v>
+      </c>
+      <c r="L17" s="74">
+        <v>1</v>
+      </c>
+      <c r="M17" s="74">
+        <v>1</v>
+      </c>
+      <c r="N17" s="80">
+        <v>0</v>
+      </c>
+      <c r="O17" s="72">
+        <v>9</v>
+      </c>
+      <c r="P17" s="73">
+        <v>3</v>
+      </c>
+      <c r="Q17" s="73">
+        <v>3</v>
+      </c>
+      <c r="R17" s="73">
+        <v>3</v>
+      </c>
+      <c r="S17" s="71">
+        <v>4</v>
+      </c>
+      <c r="T17" s="68"/>
+      <c r="U17" s="68"/>
+    </row>
+    <row r="18" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A18" s="68"/>
+      <c r="B18" s="68"/>
+      <c r="C18" s="68"/>
+      <c r="D18" s="76">
+        <v>5</v>
+      </c>
+      <c r="E18" s="76">
+        <v>5</v>
+      </c>
+      <c r="F18" s="76">
+        <v>5</v>
+      </c>
+      <c r="G18" s="78">
+        <v>8</v>
+      </c>
+      <c r="H18" s="78">
+        <v>8</v>
+      </c>
+      <c r="I18" s="78">
+        <v>8</v>
+      </c>
+      <c r="J18" s="80">
+        <v>0</v>
+      </c>
+      <c r="K18" s="80">
+        <v>0</v>
+      </c>
+      <c r="L18" s="2">
+        <v>1</v>
+      </c>
+      <c r="M18" s="2">
+        <v>1</v>
+      </c>
+      <c r="N18" s="2">
+        <v>1</v>
+      </c>
+      <c r="O18" s="72">
+        <v>9</v>
+      </c>
+      <c r="P18" s="73">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="73">
+        <v>3</v>
+      </c>
+      <c r="R18" s="73">
+        <v>3</v>
+      </c>
+      <c r="S18" s="68"/>
+      <c r="T18" s="68"/>
+      <c r="U18" s="68"/>
+    </row>
+    <row r="19" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A19" s="68"/>
+      <c r="B19" s="68"/>
+      <c r="C19" s="68"/>
+      <c r="D19" s="68"/>
+      <c r="E19" s="71">
+        <v>4</v>
+      </c>
+      <c r="F19" s="76">
+        <v>5</v>
+      </c>
+      <c r="G19" s="76">
+        <v>5</v>
+      </c>
+      <c r="H19" s="76">
+        <v>5</v>
+      </c>
+      <c r="I19" s="76">
+        <v>5</v>
+      </c>
+      <c r="J19" s="78">
+        <v>8</v>
+      </c>
+      <c r="K19" s="80">
+        <v>0</v>
+      </c>
+      <c r="L19" s="2">
+        <v>1</v>
+      </c>
+      <c r="M19" s="2">
+        <v>1</v>
+      </c>
+      <c r="N19" s="2">
+        <v>1</v>
+      </c>
+      <c r="O19" s="72">
+        <v>9</v>
+      </c>
+      <c r="P19" s="73">
+        <v>3</v>
+      </c>
+      <c r="Q19" s="71">
+        <v>4</v>
+      </c>
+      <c r="R19" s="68"/>
+      <c r="S19" s="68"/>
+      <c r="T19" s="68"/>
+      <c r="U19" s="68"/>
+    </row>
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A20" s="68"/>
+      <c r="B20" s="68"/>
+      <c r="C20" s="68"/>
+      <c r="D20" s="68"/>
+      <c r="E20" s="68"/>
+      <c r="F20" s="68"/>
+      <c r="G20" s="76">
+        <v>5</v>
+      </c>
+      <c r="H20" s="76">
+        <v>5</v>
+      </c>
+      <c r="I20" s="76">
+        <v>5</v>
+      </c>
+      <c r="J20" s="76">
+        <v>5</v>
+      </c>
+      <c r="K20" s="78">
+        <v>8</v>
+      </c>
+      <c r="L20" s="76">
+        <v>5</v>
+      </c>
+      <c r="M20" s="76">
+        <v>5</v>
+      </c>
+      <c r="N20" s="76">
+        <v>5</v>
+      </c>
+      <c r="O20" s="72">
+        <v>9</v>
+      </c>
+      <c r="P20" s="68"/>
+      <c r="Q20" s="68"/>
+      <c r="R20" s="68"/>
+      <c r="S20" s="68"/>
+      <c r="T20" s="68"/>
+      <c r="U20" s="68"/>
+    </row>
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A21" s="68"/>
+      <c r="B21" s="68"/>
+      <c r="C21" s="68"/>
+      <c r="D21" s="68"/>
+      <c r="E21" s="68"/>
+      <c r="F21" s="68"/>
+      <c r="G21" s="68"/>
+      <c r="H21" s="68"/>
+      <c r="I21" s="76">
+        <v>5</v>
+      </c>
+      <c r="J21" s="76">
+        <v>5</v>
+      </c>
+      <c r="K21" s="76">
+        <v>5</v>
+      </c>
+      <c r="L21" s="78">
+        <v>8</v>
+      </c>
+      <c r="M21" s="76">
+        <v>5</v>
+      </c>
+      <c r="N21" s="68"/>
+      <c r="O21" s="68"/>
+      <c r="P21" s="68"/>
+      <c r="Q21" s="68"/>
+      <c r="R21" s="68"/>
+      <c r="S21" s="68"/>
+      <c r="T21" s="68"/>
+      <c r="U21" s="68"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
changed the width of the converted map cells
</commit_message>
<xml_diff>
--- a/Documentation/R5 Coords.xlsx
+++ b/Documentation/R5 Coords.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orola\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Game_RPG_Adventure\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD268ABC-AA3C-4C79-B05A-C7E2BD6C3153}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94E8030B-7BE2-4BC1-AA80-FB3111459FD8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Converted to numbers" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1199,28 +1200,28 @@
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="14" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="16" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="14" borderId="0" xfId="13" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="3" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" xfId="3" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" xfId="14" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" xfId="9" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" xfId="16" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1566,30 +1567,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28" ht="33.75" customHeight="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="83" t="s">
+      <c r="A1" s="89" t="s">
         <v>92</v>
       </c>
-      <c r="B1" s="83"/>
-      <c r="C1" s="83"/>
-      <c r="D1" s="83"/>
-      <c r="E1" s="83"/>
+      <c r="B1" s="89"/>
+      <c r="C1" s="89"/>
+      <c r="D1" s="89"/>
+      <c r="E1" s="89"/>
       <c r="F1" s="81"/>
     </row>
     <row r="2" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="89" t="s">
         <v>91</v>
       </c>
-      <c r="B2" s="83"/>
-      <c r="C2" s="83"/>
-      <c r="D2" s="83"/>
-      <c r="E2" s="83"/>
-      <c r="F2" s="83"/>
-      <c r="G2" s="83"/>
-      <c r="H2" s="83"/>
-      <c r="I2" s="83"/>
-      <c r="J2" s="83"/>
-      <c r="K2" s="83"/>
-      <c r="L2" s="83"/>
+      <c r="B2" s="89"/>
+      <c r="C2" s="89"/>
+      <c r="D2" s="89"/>
+      <c r="E2" s="89"/>
+      <c r="F2" s="89"/>
+      <c r="G2" s="89"/>
+      <c r="H2" s="89"/>
+      <c r="I2" s="89"/>
+      <c r="J2" s="89"/>
+      <c r="K2" s="89"/>
+      <c r="L2" s="89"/>
     </row>
     <row r="3" spans="1:28" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="6"/>
@@ -2882,7 +2883,7 @@
       <c r="BV4" s="75">
         <v>2</v>
       </c>
-      <c r="BW4" s="88">
+      <c r="BW4" s="86">
         <v>16</v>
       </c>
       <c r="BX4" s="68"/>
@@ -3340,7 +3341,7 @@
       <c r="BH7" s="77">
         <v>5</v>
       </c>
-      <c r="BI7" s="87">
+      <c r="BI7" s="85">
         <v>101</v>
       </c>
       <c r="BJ7" s="77">
@@ -4063,7 +4064,7 @@
       <c r="BN11" s="74">
         <v>1</v>
       </c>
-      <c r="BO11" s="89">
+      <c r="BO11" s="87">
         <v>1</v>
       </c>
       <c r="BP11" s="74">
@@ -4318,7 +4319,7 @@
       <c r="BO12" s="74">
         <v>1</v>
       </c>
-      <c r="BP12" s="86">
+      <c r="BP12" s="84">
         <v>10</v>
       </c>
       <c r="BQ12" s="74">
@@ -4596,10 +4597,10 @@
       <c r="B14" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="C14" s="84" t="s">
+      <c r="C14" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="84"/>
+      <c r="D14" s="90"/>
       <c r="E14" s="78"/>
       <c r="F14" s="79"/>
       <c r="G14" s="79"/>
@@ -5188,7 +5189,7 @@
       <c r="BE17" s="68"/>
       <c r="BF17" s="68"/>
       <c r="BG17" s="68"/>
-      <c r="BH17" s="85">
+      <c r="BH17" s="83">
         <v>12</v>
       </c>
       <c r="BI17" s="76">
@@ -5227,7 +5228,7 @@
       <c r="BT17" s="72">
         <v>7</v>
       </c>
-      <c r="BU17" s="87">
+      <c r="BU17" s="85">
         <v>15</v>
       </c>
       <c r="BV17" s="73">
@@ -5361,7 +5362,7 @@
       <c r="BF18" s="68"/>
       <c r="BG18" s="68"/>
       <c r="BH18" s="68"/>
-      <c r="BI18" s="85">
+      <c r="BI18" s="83">
         <v>12</v>
       </c>
       <c r="BJ18" s="76">
@@ -5526,7 +5527,7 @@
       <c r="BG19" s="68"/>
       <c r="BH19" s="68"/>
       <c r="BI19" s="68"/>
-      <c r="BJ19" s="85">
+      <c r="BJ19" s="83">
         <v>12</v>
       </c>
       <c r="BK19" s="76">
@@ -5553,7 +5554,7 @@
       <c r="BR19" s="74">
         <v>1</v>
       </c>
-      <c r="BS19" s="90">
+      <c r="BS19" s="88">
         <v>100</v>
       </c>
       <c r="BT19" s="72">
@@ -6368,10 +6369,10 @@
       <c r="B38" s="74" t="s">
         <v>83</v>
       </c>
-      <c r="C38" s="84" t="s">
+      <c r="C38" s="90" t="s">
         <v>84</v>
       </c>
-      <c r="D38" s="84"/>
+      <c r="D38" s="90"/>
       <c r="E38" s="78"/>
       <c r="F38" s="79"/>
       <c r="G38" s="79"/>
@@ -6653,11 +6654,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:U21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="95" workbookViewId="0">
-      <selection activeCell="L35" sqref="L35"/>
+    <sheetView tabSelected="1" zoomScale="95" workbookViewId="0">
+      <selection activeCell="S18" sqref="S18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="21" width="5.7109375" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="68"/>
@@ -7810,5 +7814,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>